<commit_message>
UI changes and log template dropdown
lots of changes with the ui includingcreating a log template dropdown
</commit_message>
<xml_diff>
--- a/tops_data.xlsx
+++ b/tops_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">UWI</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t xml:space="preserve">Top2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top5</t>
   </si>
   <si>
     <t xml:space="preserve">Kennetcook2</t>
@@ -130,17 +139,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -156,19 +166,37 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>94.8</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>400</v>
+        <v>600</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>